<commit_message>
add the feature engineering code
</commit_message>
<xml_diff>
--- a/data/tname.xlsx
+++ b/data/tname.xlsx
@@ -5,22 +5,37 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/社交网络/PJ/code/mxl/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/社交网络/PJ/code/SocialNetwork_mxl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F220E22A-3B3B-164F-8D6A-B22D238CCB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7B3E18-BDFD-F94F-AC6C-B85F77F6F62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$124</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="137">
   <si>
     <t>name</t>
   </si>
@@ -390,6 +405,49 @@
   </si>
   <si>
     <t>typeid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>鬼畜</t>
+  </si>
+  <si>
+    <t>舞蹈</t>
+  </si>
+  <si>
+    <t>娱乐</t>
+  </si>
+  <si>
+    <t>科技</t>
+  </si>
+  <si>
+    <t>美食</t>
+  </si>
+  <si>
+    <t>汽车</t>
+  </si>
+  <si>
+    <t>电影</t>
+  </si>
+  <si>
+    <t>游戏</t>
+  </si>
+  <si>
+    <t>音乐</t>
+  </si>
+  <si>
+    <t>影视</t>
+  </si>
+  <si>
+    <t>知识</t>
+  </si>
+  <si>
+    <t>时尚</t>
+  </si>
+  <si>
+    <t>动物圈</t>
+  </si>
+  <si>
+    <t>cat0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -762,1008 +820,1384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B124"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E26" sqref="E22:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>124</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>228</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>164</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>162</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>183</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>76</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>161</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>218</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>137</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>184</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>185</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>85</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>168</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>138</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>171</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>71</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>95</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>122</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>158</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>157</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>250</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>174</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>215</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>208</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>256</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>59</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>249</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>209</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>205</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>182</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>28</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>254</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>239</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>213</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>212</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>238</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>236</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>180</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>176</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>251</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>172</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>193</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>31</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>159</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>130</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>29</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>220</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>207</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>17</v>
       </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>47</v>
       </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>65</v>
       </c>
       <c r="B54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55">
         <v>248</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56">
         <v>246</v>
       </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57">
         <v>258</v>
       </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58">
         <v>240</v>
       </c>
       <c r="B58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59">
         <v>210</v>
       </c>
       <c r="B59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60">
         <v>198</v>
       </c>
       <c r="B60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61">
         <v>230</v>
       </c>
       <c r="B61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62">
         <v>136</v>
       </c>
       <c r="B62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63">
         <v>237</v>
       </c>
       <c r="B63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64">
         <v>235</v>
       </c>
       <c r="B64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65">
         <v>233</v>
       </c>
       <c r="B65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66">
         <v>231</v>
       </c>
       <c r="B66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67">
         <v>201</v>
       </c>
       <c r="B67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68">
         <v>232</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69">
         <v>154</v>
       </c>
       <c r="B69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="C69" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70">
         <v>252</v>
       </c>
       <c r="B70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="C70" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71">
         <v>222</v>
       </c>
       <c r="B71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72">
         <v>20</v>
       </c>
       <c r="B72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73">
         <v>243</v>
       </c>
       <c r="B73" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="C73" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74">
         <v>22</v>
       </c>
       <c r="B74" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="C74" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75">
         <v>216</v>
       </c>
       <c r="B75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="C75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76">
         <v>170</v>
       </c>
       <c r="B76" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="C76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77">
         <v>253</v>
       </c>
       <c r="B77" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="C77" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78">
         <v>24</v>
       </c>
       <c r="B78" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="C78" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79">
         <v>173</v>
       </c>
       <c r="B79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="C79" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80">
         <v>247</v>
       </c>
       <c r="B80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="C80" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81">
         <v>199</v>
       </c>
       <c r="B81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="C81" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82">
         <v>30</v>
       </c>
       <c r="B82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="C82" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83">
         <v>257</v>
       </c>
       <c r="B83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="C83" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84">
         <v>86</v>
       </c>
       <c r="B84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="C84" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85">
         <v>19</v>
       </c>
       <c r="B85" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="C85" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86">
         <v>244</v>
       </c>
       <c r="B86" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="C86" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87">
         <v>203</v>
       </c>
       <c r="B87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="C87" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88">
         <v>242</v>
       </c>
       <c r="B88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="C88" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89">
         <v>245</v>
       </c>
       <c r="B89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="C89" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90">
         <v>227</v>
       </c>
       <c r="B90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="C90" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
       <c r="A91">
         <v>229</v>
       </c>
       <c r="B91" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="C91" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92">
         <v>37</v>
       </c>
       <c r="B92" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="C92" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93">
         <v>121</v>
       </c>
       <c r="B93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="C93" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94">
         <v>75</v>
       </c>
       <c r="B94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="C94" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
       <c r="A95">
         <v>214</v>
       </c>
       <c r="B95" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="C95" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96">
         <v>219</v>
       </c>
       <c r="B96" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="C96" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97">
         <v>178</v>
       </c>
       <c r="B97" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="C97" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98">
         <v>255</v>
       </c>
       <c r="B98" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="C98" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99">
         <v>200</v>
       </c>
       <c r="B99" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="C99" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100">
         <v>26</v>
       </c>
       <c r="B100" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="C100" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101">
         <v>126</v>
       </c>
       <c r="B101" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="C101" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102">
         <v>25</v>
       </c>
       <c r="B102" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="C102" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103">
         <v>179</v>
       </c>
       <c r="B103" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="C103" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104">
         <v>156</v>
       </c>
       <c r="B104" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="C104" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105">
         <v>221</v>
       </c>
       <c r="B105" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="C105" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106">
         <v>153</v>
       </c>
       <c r="B106" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="C106" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107">
         <v>241</v>
       </c>
       <c r="B107" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:2">
+      <c r="C107" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108">
         <v>204</v>
       </c>
       <c r="B108" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:2">
+      <c r="C108" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109">
         <v>206</v>
       </c>
       <c r="B109" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="110" spans="1:2">
+      <c r="C109" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110">
         <v>152</v>
       </c>
       <c r="B110" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="111" spans="1:2">
+      <c r="C110" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111">
         <v>195</v>
       </c>
       <c r="B111" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="112" spans="1:2">
+      <c r="C111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112">
         <v>1</v>
       </c>
       <c r="B112" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="113" spans="1:2">
+      <c r="C112" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113">
         <v>51</v>
       </c>
       <c r="B113" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="114" spans="1:2">
+      <c r="C113" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114">
         <v>127</v>
       </c>
       <c r="B114" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="115" spans="1:2">
+      <c r="C114" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
       <c r="A115">
         <v>32</v>
       </c>
       <c r="B115" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="116" spans="1:2">
+      <c r="C115" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
       <c r="A116">
         <v>33</v>
       </c>
       <c r="B116" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="117" spans="1:2">
+      <c r="C116" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
       <c r="A117">
         <v>145</v>
       </c>
       <c r="B117" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="118" spans="1:2">
+      <c r="C117" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118">
         <v>54</v>
       </c>
       <c r="B118" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="119" spans="1:2">
+      <c r="C118" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
       <c r="A119">
         <v>187</v>
       </c>
       <c r="B119" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="120" spans="1:2">
+      <c r="C119" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
       <c r="A120">
         <v>147</v>
       </c>
       <c r="B120" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="121" spans="1:2">
+      <c r="C120" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
       <c r="A121">
         <v>169</v>
       </c>
       <c r="B121" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="122" spans="1:2">
+      <c r="C121" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
       <c r="A122">
         <v>39</v>
       </c>
       <c r="B122" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="123" spans="1:2">
+      <c r="C122" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
       <c r="A123">
         <v>163</v>
       </c>
       <c r="B123" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="124" spans="1:2">
+      <c r="C123" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
       <c r="A124">
         <v>160</v>
       </c>
       <c r="B124" t="s">
+        <v>120</v>
+      </c>
+      <c r="C124" t="s">
         <v>120</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>